<commit_message>
This is my 1st commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="118">
   <si>
     <t>Package Name</t>
   </si>
@@ -1958,7 +1958,9 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>

</xml_diff>